<commit_message>
Utilizando Delimitadores e Arrumando a Base
</commit_message>
<xml_diff>
--- a/3-Classificar_e_filtrar/08. Filtro Avançado (Parte 3) - Material(1).xlsx
+++ b/3-Classificar_e_filtrar/08. Filtro Avançado (Parte 3) - Material(1).xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaof\Desktop\Excel Impressionador 2021\Módulo 6 - Classificar e Filtrar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\cursos\excel\3-Classificar_e_filtrar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1B6D9C-3696-4901-82AF-BF6ED43FBDB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3010F929-12E4-48F9-A7A3-98AF6E526A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{C6E87BD6-FE14-4974-BC6A-7B7E1C7A212E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{C6E87BD6-FE14-4974-BC6A-7B7E1C7A212E}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
+    <sheet name="Vendedores" sheetId="3" r:id="rId2"/>
+    <sheet name="Resultado" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Base!$A$7:$D$366</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="0">Base!$G$7</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="2">Resultado!$A$1:$B$1</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="1">Vendedores!$A$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="16">
   <si>
     <t>Vendedor</t>
   </si>
@@ -118,7 +123,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -137,6 +142,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -150,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -169,6 +180,8 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -187,9 +200,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -227,7 +240,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -333,7 +346,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -475,7 +488,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -485,60 +498,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D406A8DD-58A6-4CCB-B11F-7AE90C3A6DA2}">
   <dimension ref="A1:J366"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="16.33203125" style="2" customWidth="1"/>
-    <col min="5" max="6" width="9" customWidth="1"/>
-    <col min="7" max="10" width="12.6640625" customWidth="1"/>
+    <col min="1" max="4" width="16.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>11</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B2"/>
       <c r="C2"/>
       <c r="D2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
@@ -551,12 +565,11 @@
       <c r="D7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G7" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>44197</v>
       </c>
@@ -569,12 +582,11 @@
       <c r="D8" s="5">
         <v>5400</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G8" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>44197</v>
       </c>
@@ -587,12 +599,11 @@
       <c r="D9" s="5">
         <v>1200</v>
       </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G9" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>44198</v>
       </c>
@@ -605,12 +616,11 @@
       <c r="D10" s="5">
         <v>5400</v>
       </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G10" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>44198</v>
       </c>
@@ -623,12 +633,11 @@
       <c r="D11" s="5">
         <v>2500</v>
       </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="5"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G11" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>44198</v>
       </c>
@@ -641,12 +650,11 @@
       <c r="D12" s="5">
         <v>5400</v>
       </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="5"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G12" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>44198</v>
       </c>
@@ -659,12 +667,11 @@
       <c r="D13" s="5">
         <v>8000</v>
       </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="5"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G13" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>44200</v>
       </c>
@@ -677,12 +684,8 @@
       <c r="D14" s="5">
         <v>5400</v>
       </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="5"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>44200</v>
       </c>
@@ -695,12 +698,8 @@
       <c r="D15" s="5">
         <v>8000</v>
       </c>
-      <c r="G15" s="4"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>44200</v>
       </c>
@@ -713,12 +712,8 @@
       <c r="D16" s="5">
         <v>5400</v>
       </c>
-      <c r="G16" s="4"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="5"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>44202</v>
       </c>
@@ -731,12 +726,8 @@
       <c r="D17" s="5">
         <v>2500</v>
       </c>
-      <c r="G17" s="4"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="5"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>44202</v>
       </c>
@@ -749,12 +740,8 @@
       <c r="D18" s="5">
         <v>5400</v>
       </c>
-      <c r="G18" s="4"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="5"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>44203</v>
       </c>
@@ -768,12 +755,8 @@
         <v>1200</v>
       </c>
       <c r="F19" s="1"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="5"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>44203</v>
       </c>
@@ -788,7 +771,7 @@
       </c>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>44205</v>
       </c>
@@ -802,7 +785,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>44205</v>
       </c>
@@ -816,7 +799,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>44206</v>
       </c>
@@ -830,7 +813,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>44206</v>
       </c>
@@ -844,7 +827,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>44208</v>
       </c>
@@ -858,7 +841,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>44209</v>
       </c>
@@ -872,7 +855,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>44209</v>
       </c>
@@ -886,7 +869,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>44210</v>
       </c>
@@ -900,7 +883,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>44210</v>
       </c>
@@ -914,7 +897,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>44210</v>
       </c>
@@ -928,7 +911,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>44210</v>
       </c>
@@ -942,7 +925,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>44210</v>
       </c>
@@ -956,7 +939,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>44212</v>
       </c>
@@ -970,7 +953,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>44214</v>
       </c>
@@ -984,7 +967,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>44215</v>
       </c>
@@ -998,7 +981,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>44215</v>
       </c>
@@ -1012,7 +995,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>44216</v>
       </c>
@@ -1026,7 +1009,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>44216</v>
       </c>
@@ -1040,7 +1023,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>44217</v>
       </c>
@@ -1054,7 +1037,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>44217</v>
       </c>
@@ -1068,7 +1051,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>44218</v>
       </c>
@@ -1082,7 +1065,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>44218</v>
       </c>
@@ -1096,7 +1079,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>44218</v>
       </c>
@@ -1110,7 +1093,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>44219</v>
       </c>
@@ -1124,7 +1107,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>44220</v>
       </c>
@@ -1138,7 +1121,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>44221</v>
       </c>
@@ -1152,7 +1135,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>44221</v>
       </c>
@@ -1166,7 +1149,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>44221</v>
       </c>
@@ -1180,7 +1163,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>44222</v>
       </c>
@@ -1194,7 +1177,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>44222</v>
       </c>
@@ -1208,7 +1191,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>44223</v>
       </c>
@@ -1222,7 +1205,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>44223</v>
       </c>
@@ -1236,7 +1219,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>44224</v>
       </c>
@@ -1250,7 +1233,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>44224</v>
       </c>
@@ -1264,7 +1247,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>44224</v>
       </c>
@@ -1278,7 +1261,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>44224</v>
       </c>
@@ -1292,7 +1275,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>44225</v>
       </c>
@@ -1306,7 +1289,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>44227</v>
       </c>
@@ -1320,7 +1303,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>44227</v>
       </c>
@@ -1334,7 +1317,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>44229</v>
       </c>
@@ -1348,7 +1331,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <v>44230</v>
       </c>
@@ -1362,7 +1345,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>44230</v>
       </c>
@@ -1376,7 +1359,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>44231</v>
       </c>
@@ -1390,7 +1373,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>44231</v>
       </c>
@@ -1404,7 +1387,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>44231</v>
       </c>
@@ -1418,7 +1401,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>44232</v>
       </c>
@@ -1432,7 +1415,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>44232</v>
       </c>
@@ -1446,7 +1429,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>44232</v>
       </c>
@@ -1460,7 +1443,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <v>44232</v>
       </c>
@@ -1474,7 +1457,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <v>44232</v>
       </c>
@@ -1488,7 +1471,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
         <v>44232</v>
       </c>
@@ -1502,7 +1485,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <v>44233</v>
       </c>
@@ -1516,7 +1499,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
         <v>44233</v>
       </c>
@@ -1530,7 +1513,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
         <v>44233</v>
       </c>
@@ -1544,7 +1527,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
         <v>44234</v>
       </c>
@@ -1558,7 +1541,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
         <v>44235</v>
       </c>
@@ -1572,7 +1555,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <v>44235</v>
       </c>
@@ -1586,7 +1569,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
         <v>44235</v>
       </c>
@@ -1600,7 +1583,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
         <v>44235</v>
       </c>
@@ -1614,7 +1597,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
         <v>44236</v>
       </c>
@@ -1628,7 +1611,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
         <v>44236</v>
       </c>
@@ -1642,7 +1625,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <v>44236</v>
       </c>
@@ -1656,7 +1639,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
         <v>44238</v>
       </c>
@@ -1670,7 +1653,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
         <v>44239</v>
       </c>
@@ -1684,7 +1667,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
         <v>44239</v>
       </c>
@@ -1698,7 +1681,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
         <v>44239</v>
       </c>
@@ -1712,7 +1695,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
         <v>44239</v>
       </c>
@@ -1726,7 +1709,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="4">
         <v>44239</v>
       </c>
@@ -1740,7 +1723,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
         <v>44239</v>
       </c>
@@ -1754,7 +1737,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="4">
         <v>44240</v>
       </c>
@@ -1768,7 +1751,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="4">
         <v>44240</v>
       </c>
@@ -1782,7 +1765,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
         <v>44241</v>
       </c>
@@ -1796,7 +1779,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="4">
         <v>44241</v>
       </c>
@@ -1810,7 +1793,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
         <v>44242</v>
       </c>
@@ -1824,7 +1807,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="4">
         <v>44243</v>
       </c>
@@ -1838,7 +1821,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="4">
         <v>44244</v>
       </c>
@@ -1852,7 +1835,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="4">
         <v>44245</v>
       </c>
@@ -1866,7 +1849,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="4">
         <v>44245</v>
       </c>
@@ -1880,7 +1863,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="4">
         <v>44245</v>
       </c>
@@ -1894,7 +1877,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="4">
         <v>44248</v>
       </c>
@@ -1908,7 +1891,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="4">
         <v>44248</v>
       </c>
@@ -1922,7 +1905,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="4">
         <v>44248</v>
       </c>
@@ -1936,7 +1919,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="4">
         <v>44249</v>
       </c>
@@ -1950,7 +1933,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="4">
         <v>44249</v>
       </c>
@@ -1964,7 +1947,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="4">
         <v>44249</v>
       </c>
@@ -1978,7 +1961,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="4">
         <v>44251</v>
       </c>
@@ -1992,7 +1975,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="4">
         <v>44251</v>
       </c>
@@ -2006,7 +1989,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="4">
         <v>44253</v>
       </c>
@@ -2020,7 +2003,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="4">
         <v>44254</v>
       </c>
@@ -2034,7 +2017,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="4">
         <v>44255</v>
       </c>
@@ -2048,7 +2031,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="4">
         <v>44256</v>
       </c>
@@ -2062,7 +2045,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="4">
         <v>44257</v>
       </c>
@@ -2076,7 +2059,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="4">
         <v>44258</v>
       </c>
@@ -2090,7 +2073,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="4">
         <v>44258</v>
       </c>
@@ -2104,7 +2087,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="4">
         <v>44259</v>
       </c>
@@ -2118,7 +2101,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="4">
         <v>44260</v>
       </c>
@@ -2132,7 +2115,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="4">
         <v>44260</v>
       </c>
@@ -2146,7 +2129,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="4">
         <v>44260</v>
       </c>
@@ -2160,7 +2143,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="4">
         <v>44260</v>
       </c>
@@ -2174,7 +2157,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="4">
         <v>44261</v>
       </c>
@@ -2188,7 +2171,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="4">
         <v>44261</v>
       </c>
@@ -2202,7 +2185,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="4">
         <v>44261</v>
       </c>
@@ -2216,7 +2199,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="4">
         <v>44261</v>
       </c>
@@ -2230,7 +2213,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="4">
         <v>44262</v>
       </c>
@@ -2244,7 +2227,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="4">
         <v>44263</v>
       </c>
@@ -2258,7 +2241,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="4">
         <v>44264</v>
       </c>
@@ -2272,7 +2255,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="4">
         <v>44265</v>
       </c>
@@ -2286,7 +2269,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="4">
         <v>44265</v>
       </c>
@@ -2300,7 +2283,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="4">
         <v>44265</v>
       </c>
@@ -2314,7 +2297,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="4">
         <v>44265</v>
       </c>
@@ -2328,7 +2311,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="4">
         <v>44266</v>
       </c>
@@ -2342,7 +2325,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="4">
         <v>44267</v>
       </c>
@@ -2356,7 +2339,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="4">
         <v>44267</v>
       </c>
@@ -2370,7 +2353,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="4">
         <v>44268</v>
       </c>
@@ -2384,7 +2367,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="4">
         <v>44268</v>
       </c>
@@ -2398,7 +2381,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="4">
         <v>44269</v>
       </c>
@@ -2412,7 +2395,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="4">
         <v>44269</v>
       </c>
@@ -2426,7 +2409,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="4">
         <v>44270</v>
       </c>
@@ -2440,7 +2423,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="4">
         <v>44270</v>
       </c>
@@ -2454,7 +2437,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="4">
         <v>44270</v>
       </c>
@@ -2468,7 +2451,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="4">
         <v>44270</v>
       </c>
@@ -2482,7 +2465,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="4">
         <v>44271</v>
       </c>
@@ -2496,7 +2479,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="4">
         <v>44271</v>
       </c>
@@ -2510,7 +2493,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="4">
         <v>44272</v>
       </c>
@@ -2524,7 +2507,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="4">
         <v>44273</v>
       </c>
@@ -2538,7 +2521,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="4">
         <v>44273</v>
       </c>
@@ -2552,7 +2535,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="4">
         <v>44273</v>
       </c>
@@ -2566,7 +2549,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="4">
         <v>44274</v>
       </c>
@@ -2580,7 +2563,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="4">
         <v>44274</v>
       </c>
@@ -2594,7 +2577,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="4">
         <v>44276</v>
       </c>
@@ -2608,7 +2591,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="4">
         <v>44276</v>
       </c>
@@ -2622,7 +2605,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="4">
         <v>44277</v>
       </c>
@@ -2636,7 +2619,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="4">
         <v>44277</v>
       </c>
@@ -2650,7 +2633,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="4">
         <v>44277</v>
       </c>
@@ -2664,7 +2647,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="4">
         <v>44277</v>
       </c>
@@ -2678,7 +2661,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="4">
         <v>44277</v>
       </c>
@@ -2692,7 +2675,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="4">
         <v>44278</v>
       </c>
@@ -2706,7 +2689,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="4">
         <v>44280</v>
       </c>
@@ -2720,7 +2703,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="4">
         <v>44280</v>
       </c>
@@ -2734,7 +2717,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="4">
         <v>44280</v>
       </c>
@@ -2748,7 +2731,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="4">
         <v>44281</v>
       </c>
@@ -2762,7 +2745,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="4">
         <v>44282</v>
       </c>
@@ -2776,7 +2759,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="4">
         <v>44283</v>
       </c>
@@ -2790,7 +2773,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="4">
         <v>44283</v>
       </c>
@@ -2804,7 +2787,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="4">
         <v>44284</v>
       </c>
@@ -2818,7 +2801,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="4">
         <v>44284</v>
       </c>
@@ -2832,7 +2815,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="4">
         <v>44285</v>
       </c>
@@ -2846,7 +2829,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="4">
         <v>44285</v>
       </c>
@@ -2860,7 +2843,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="4">
         <v>44285</v>
       </c>
@@ -2874,7 +2857,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="4">
         <v>44285</v>
       </c>
@@ -2888,7 +2871,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="4">
         <v>44286</v>
       </c>
@@ -2902,7 +2885,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="4">
         <v>44286</v>
       </c>
@@ -2916,7 +2899,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="4">
         <v>44286</v>
       </c>
@@ -2930,7 +2913,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="4">
         <v>44287</v>
       </c>
@@ -2944,7 +2927,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="4">
         <v>44288</v>
       </c>
@@ -2958,7 +2941,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="4">
         <v>44288</v>
       </c>
@@ -2972,7 +2955,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="4">
         <v>44288</v>
       </c>
@@ -2986,7 +2969,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="4">
         <v>44288</v>
       </c>
@@ -3000,7 +2983,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="4">
         <v>44289</v>
       </c>
@@ -3014,7 +2997,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="4">
         <v>44290</v>
       </c>
@@ -3028,7 +3011,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="4">
         <v>44290</v>
       </c>
@@ -3042,7 +3025,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="4">
         <v>44291</v>
       </c>
@@ -3056,7 +3039,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="4">
         <v>44291</v>
       </c>
@@ -3070,7 +3053,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="4">
         <v>44292</v>
       </c>
@@ -3084,7 +3067,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="4">
         <v>44292</v>
       </c>
@@ -3098,7 +3081,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="4">
         <v>44293</v>
       </c>
@@ -3112,7 +3095,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="4">
         <v>44293</v>
       </c>
@@ -3126,7 +3109,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="4">
         <v>44293</v>
       </c>
@@ -3140,7 +3123,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="4">
         <v>44294</v>
       </c>
@@ -3154,7 +3137,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="4">
         <v>44294</v>
       </c>
@@ -3168,7 +3151,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="4">
         <v>44295</v>
       </c>
@@ -3182,7 +3165,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="4">
         <v>44295</v>
       </c>
@@ -3196,7 +3179,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" s="4">
         <v>44295</v>
       </c>
@@ -3210,7 +3193,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="4">
         <v>44295</v>
       </c>
@@ -3224,7 +3207,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" s="4">
         <v>44296</v>
       </c>
@@ -3238,7 +3221,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="4">
         <v>44296</v>
       </c>
@@ -3252,7 +3235,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="4">
         <v>44297</v>
       </c>
@@ -3266,7 +3249,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="4">
         <v>44297</v>
       </c>
@@ -3280,7 +3263,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" s="4">
         <v>44298</v>
       </c>
@@ -3294,7 +3277,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="4">
         <v>44298</v>
       </c>
@@ -3308,7 +3291,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" s="4">
         <v>44299</v>
       </c>
@@ -3322,7 +3305,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" s="4">
         <v>44300</v>
       </c>
@@ -3336,7 +3319,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" s="4">
         <v>44300</v>
       </c>
@@ -3350,7 +3333,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" s="4">
         <v>44300</v>
       </c>
@@ -3364,7 +3347,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" s="4">
         <v>44301</v>
       </c>
@@ -3378,7 +3361,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" s="4">
         <v>44302</v>
       </c>
@@ -3392,7 +3375,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" s="4">
         <v>44302</v>
       </c>
@@ -3406,7 +3389,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" s="4">
         <v>44302</v>
       </c>
@@ -3420,7 +3403,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" s="4">
         <v>44302</v>
       </c>
@@ -3434,7 +3417,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" s="4">
         <v>44303</v>
       </c>
@@ -3448,7 +3431,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" s="4">
         <v>44303</v>
       </c>
@@ -3462,7 +3445,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" s="4">
         <v>44303</v>
       </c>
@@ -3476,7 +3459,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" s="4">
         <v>44304</v>
       </c>
@@ -3490,7 +3473,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" s="4">
         <v>44304</v>
       </c>
@@ -3504,7 +3487,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" s="4">
         <v>44306</v>
       </c>
@@ -3518,7 +3501,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" s="4">
         <v>44307</v>
       </c>
@@ -3532,7 +3515,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" s="4">
         <v>44307</v>
       </c>
@@ -3546,7 +3529,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" s="4">
         <v>44307</v>
       </c>
@@ -3560,7 +3543,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" s="4">
         <v>44308</v>
       </c>
@@ -3574,7 +3557,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" s="4">
         <v>44309</v>
       </c>
@@ -3588,7 +3571,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" s="4">
         <v>44309</v>
       </c>
@@ -3602,7 +3585,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" s="4">
         <v>44310</v>
       </c>
@@ -3616,7 +3599,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" s="4">
         <v>44310</v>
       </c>
@@ -3630,7 +3613,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" s="4">
         <v>44314</v>
       </c>
@@ -3644,7 +3627,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" s="4">
         <v>44315</v>
       </c>
@@ -3658,7 +3641,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" s="4">
         <v>44316</v>
       </c>
@@ -3672,7 +3655,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" s="4">
         <v>44317</v>
       </c>
@@ -3686,7 +3669,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" s="4">
         <v>44317</v>
       </c>
@@ -3700,7 +3683,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" s="4">
         <v>44318</v>
       </c>
@@ -3714,7 +3697,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" s="4">
         <v>44318</v>
       </c>
@@ -3728,7 +3711,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" s="4">
         <v>44319</v>
       </c>
@@ -3742,7 +3725,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" s="4">
         <v>44319</v>
       </c>
@@ -3756,7 +3739,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" s="4">
         <v>44320</v>
       </c>
@@ -3770,7 +3753,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" s="4">
         <v>44320</v>
       </c>
@@ -3784,7 +3767,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" s="4">
         <v>44320</v>
       </c>
@@ -3798,7 +3781,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" s="4">
         <v>44321</v>
       </c>
@@ -3812,7 +3795,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" s="4">
         <v>44322</v>
       </c>
@@ -3826,7 +3809,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" s="4">
         <v>44322</v>
       </c>
@@ -3840,7 +3823,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239" s="4">
         <v>44324</v>
       </c>
@@ -3854,7 +3837,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A240" s="4">
         <v>44324</v>
       </c>
@@ -3868,7 +3851,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" s="4">
         <v>44324</v>
       </c>
@@ -3882,7 +3865,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" s="4">
         <v>44324</v>
       </c>
@@ -3896,7 +3879,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" s="4">
         <v>44325</v>
       </c>
@@ -3910,7 +3893,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A244" s="4">
         <v>44326</v>
       </c>
@@ -3924,7 +3907,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245" s="4">
         <v>44326</v>
       </c>
@@ -3938,7 +3921,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" s="4">
         <v>44327</v>
       </c>
@@ -3952,7 +3935,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" s="4">
         <v>44327</v>
       </c>
@@ -3966,7 +3949,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" s="4">
         <v>44328</v>
       </c>
@@ -3980,7 +3963,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A249" s="4">
         <v>44328</v>
       </c>
@@ -3994,7 +3977,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" s="4">
         <v>44329</v>
       </c>
@@ -4008,7 +3991,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" s="4">
         <v>44329</v>
       </c>
@@ -4022,7 +4005,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" s="4">
         <v>44329</v>
       </c>
@@ -4036,7 +4019,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" s="4">
         <v>44330</v>
       </c>
@@ -4050,7 +4033,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" s="4">
         <v>44331</v>
       </c>
@@ -4064,7 +4047,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A255" s="4">
         <v>44331</v>
       </c>
@@ -4078,7 +4061,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" s="4">
         <v>44332</v>
       </c>
@@ -4092,7 +4075,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257" s="4">
         <v>44332</v>
       </c>
@@ -4106,7 +4089,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" s="4">
         <v>44333</v>
       </c>
@@ -4120,7 +4103,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" s="4">
         <v>44333</v>
       </c>
@@ -4134,7 +4117,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" s="4">
         <v>44336</v>
       </c>
@@ -4148,7 +4131,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" s="4">
         <v>44337</v>
       </c>
@@ -4162,7 +4145,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" s="4">
         <v>44337</v>
       </c>
@@ -4176,7 +4159,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" s="4">
         <v>44338</v>
       </c>
@@ -4190,7 +4173,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" s="4">
         <v>44338</v>
       </c>
@@ -4204,7 +4187,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A265" s="4">
         <v>44338</v>
       </c>
@@ -4218,7 +4201,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" s="4">
         <v>44338</v>
       </c>
@@ -4232,7 +4215,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A267" s="4">
         <v>44339</v>
       </c>
@@ -4246,7 +4229,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A268" s="4">
         <v>44339</v>
       </c>
@@ -4260,7 +4243,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269" s="4">
         <v>44340</v>
       </c>
@@ -4274,7 +4257,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270" s="4">
         <v>44340</v>
       </c>
@@ -4288,7 +4271,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A271" s="4">
         <v>44341</v>
       </c>
@@ -4302,7 +4285,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="272" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A272" s="4">
         <v>44341</v>
       </c>
@@ -4316,7 +4299,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A273" s="4">
         <v>44341</v>
       </c>
@@ -4330,7 +4313,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A274" s="4">
         <v>44342</v>
       </c>
@@ -4344,7 +4327,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A275" s="4">
         <v>44342</v>
       </c>
@@ -4358,7 +4341,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="276" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A276" s="4">
         <v>44342</v>
       </c>
@@ -4372,7 +4355,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A277" s="4">
         <v>44342</v>
       </c>
@@ -4386,7 +4369,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A278" s="4">
         <v>44344</v>
       </c>
@@ -4400,7 +4383,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A279" s="4">
         <v>44344</v>
       </c>
@@ -4414,7 +4397,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="280" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A280" s="4">
         <v>44344</v>
       </c>
@@ -4428,7 +4411,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="281" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A281" s="4">
         <v>44345</v>
       </c>
@@ -4442,7 +4425,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="282" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A282" s="4">
         <v>44347</v>
       </c>
@@ -4456,7 +4439,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="283" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A283" s="4">
         <v>44347</v>
       </c>
@@ -4470,7 +4453,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="284" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A284" s="4">
         <v>44347</v>
       </c>
@@ -4484,7 +4467,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="285" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A285" s="4">
         <v>44347</v>
       </c>
@@ -4498,7 +4481,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="286" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A286" s="4">
         <v>44347</v>
       </c>
@@ -4512,7 +4495,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="287" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A287" s="4">
         <v>44348</v>
       </c>
@@ -4526,7 +4509,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="288" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A288" s="4">
         <v>44348</v>
       </c>
@@ -4540,7 +4523,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A289" s="4">
         <v>44349</v>
       </c>
@@ -4554,7 +4537,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A290" s="4">
         <v>44351</v>
       </c>
@@ -4568,7 +4551,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A291" s="4">
         <v>44352</v>
       </c>
@@ -4582,7 +4565,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A292" s="4">
         <v>44353</v>
       </c>
@@ -4596,7 +4579,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A293" s="4">
         <v>44354</v>
       </c>
@@ -4610,7 +4593,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A294" s="4">
         <v>44354</v>
       </c>
@@ -4624,7 +4607,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A295" s="4">
         <v>44355</v>
       </c>
@@ -4638,7 +4621,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A296" s="4">
         <v>44356</v>
       </c>
@@ -4652,7 +4635,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A297" s="4">
         <v>44357</v>
       </c>
@@ -4666,7 +4649,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A298" s="4">
         <v>44357</v>
       </c>
@@ -4680,7 +4663,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A299" s="4">
         <v>44357</v>
       </c>
@@ -4694,7 +4677,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A300" s="4">
         <v>44357</v>
       </c>
@@ -4708,7 +4691,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A301" s="4">
         <v>44358</v>
       </c>
@@ -4722,7 +4705,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A302" s="4">
         <v>44358</v>
       </c>
@@ -4736,7 +4719,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="303" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A303" s="4">
         <v>44359</v>
       </c>
@@ -4750,7 +4733,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="304" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A304" s="4">
         <v>44359</v>
       </c>
@@ -4764,7 +4747,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A305" s="4">
         <v>44360</v>
       </c>
@@ -4778,7 +4761,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="306" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A306" s="4">
         <v>44360</v>
       </c>
@@ -4792,7 +4775,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="307" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A307" s="4">
         <v>44361</v>
       </c>
@@ -4806,7 +4789,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A308" s="4">
         <v>44361</v>
       </c>
@@ -4820,7 +4803,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A309" s="4">
         <v>44362</v>
       </c>
@@ -4834,7 +4817,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A310" s="4">
         <v>44362</v>
       </c>
@@ -4848,7 +4831,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A311" s="4">
         <v>44362</v>
       </c>
@@ -4862,7 +4845,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="312" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A312" s="4">
         <v>44362</v>
       </c>
@@ -4876,7 +4859,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="313" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A313" s="4">
         <v>44364</v>
       </c>
@@ -4890,7 +4873,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="314" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A314" s="4">
         <v>44364</v>
       </c>
@@ -4904,7 +4887,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="315" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A315" s="4">
         <v>44364</v>
       </c>
@@ -4918,7 +4901,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="316" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A316" s="4">
         <v>44365</v>
       </c>
@@ -4932,7 +4915,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="317" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A317" s="4">
         <v>44365</v>
       </c>
@@ -4946,7 +4929,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="318" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A318" s="4">
         <v>44365</v>
       </c>
@@ -4960,7 +4943,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="319" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A319" s="4">
         <v>44366</v>
       </c>
@@ -4974,7 +4957,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="320" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A320" s="4">
         <v>44366</v>
       </c>
@@ -4988,7 +4971,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="321" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A321" s="4">
         <v>44367</v>
       </c>
@@ -5002,7 +4985,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="322" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A322" s="4">
         <v>44367</v>
       </c>
@@ -5016,7 +4999,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="323" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A323" s="4">
         <v>44368</v>
       </c>
@@ -5030,7 +5013,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="324" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A324" s="4">
         <v>44369</v>
       </c>
@@ -5044,7 +5027,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="325" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A325" s="4">
         <v>44369</v>
       </c>
@@ -5058,7 +5041,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="326" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A326" s="4">
         <v>44369</v>
       </c>
@@ -5072,7 +5055,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="327" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A327" s="4">
         <v>44369</v>
       </c>
@@ -5086,7 +5069,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="328" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A328" s="4">
         <v>44371</v>
       </c>
@@ -5100,7 +5083,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="329" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A329" s="4">
         <v>44372</v>
       </c>
@@ -5114,7 +5097,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="330" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A330" s="4">
         <v>44372</v>
       </c>
@@ -5128,7 +5111,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="331" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A331" s="4">
         <v>44372</v>
       </c>
@@ -5142,7 +5125,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="332" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A332" s="4">
         <v>44372</v>
       </c>
@@ -5156,7 +5139,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="333" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A333" s="4">
         <v>44372</v>
       </c>
@@ -5170,7 +5153,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="334" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A334" s="4">
         <v>44372</v>
       </c>
@@ -5184,7 +5167,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="335" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A335" s="4">
         <v>44374</v>
       </c>
@@ -5198,7 +5181,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="336" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A336" s="4">
         <v>44374</v>
       </c>
@@ -5212,7 +5195,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="337" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A337" s="4">
         <v>44374</v>
       </c>
@@ -5226,7 +5209,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="338" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A338" s="4">
         <v>44376</v>
       </c>
@@ -5240,7 +5223,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="339" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A339" s="4">
         <v>44376</v>
       </c>
@@ -5254,7 +5237,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="340" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A340" s="4">
         <v>44377</v>
       </c>
@@ -5268,7 +5251,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="341" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A341" s="4">
         <v>44378</v>
       </c>
@@ -5282,7 +5265,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="342" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A342" s="4">
         <v>44379</v>
       </c>
@@ -5296,7 +5279,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="343" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A343" s="4">
         <v>44380</v>
       </c>
@@ -5310,7 +5293,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="344" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A344" s="4">
         <v>44381</v>
       </c>
@@ -5324,7 +5307,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="345" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A345" s="4">
         <v>44383</v>
       </c>
@@ -5338,7 +5321,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="346" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A346" s="4">
         <v>44383</v>
       </c>
@@ -5352,7 +5335,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="347" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A347" s="4">
         <v>44383</v>
       </c>
@@ -5366,7 +5349,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="348" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A348" s="4">
         <v>44383</v>
       </c>
@@ -5380,7 +5363,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="349" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A349" s="4">
         <v>44384</v>
       </c>
@@ -5394,7 +5377,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="350" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A350" s="4">
         <v>44384</v>
       </c>
@@ -5408,7 +5391,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="351" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A351" s="4">
         <v>44384</v>
       </c>
@@ -5422,7 +5405,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="352" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A352" s="4">
         <v>44384</v>
       </c>
@@ -5436,7 +5419,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="353" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A353" s="4">
         <v>44384</v>
       </c>
@@ -5450,7 +5433,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="354" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A354" s="4">
         <v>44386</v>
       </c>
@@ -5464,7 +5447,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="355" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A355" s="4">
         <v>44386</v>
       </c>
@@ -5478,7 +5461,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="356" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A356" s="4">
         <v>44386</v>
       </c>
@@ -5492,7 +5475,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="357" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A357" s="4">
         <v>44386</v>
       </c>
@@ -5506,7 +5489,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="358" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A358" s="4">
         <v>44387</v>
       </c>
@@ -5520,7 +5503,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="359" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A359" s="4">
         <v>44387</v>
       </c>
@@ -5534,7 +5517,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="360" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A360" s="4">
         <v>44388</v>
       </c>
@@ -5548,7 +5531,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="361" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A361" s="4">
         <v>44389</v>
       </c>
@@ -5562,7 +5545,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="362" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A362" s="4">
         <v>44389</v>
       </c>
@@ -5576,7 +5559,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="363" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A363" s="4">
         <v>44390</v>
       </c>
@@ -5590,7 +5573,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="364" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A364" s="4">
         <v>44390</v>
       </c>
@@ -5604,7 +5587,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="365" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A365" s="4">
         <v>44391</v>
       </c>
@@ -5618,7 +5601,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="366" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A366" s="4">
         <v>44391</v>
       </c>
@@ -5636,4 +5619,1136 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F287F20-CDB6-42A8-9C55-00444E83BC22}">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF264816-1AA2-4468-95FF-1B1C3D729000}">
+  <dimension ref="A1:B133"/>
+  <sheetViews>
+    <sheetView topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B133"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="5">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="5">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="5">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="5">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="5">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="5">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="5">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="5">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="5">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="5">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="5">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="5">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="5">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="5">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="5">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="5">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="5">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="5">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="5">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35" s="5">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36" s="5">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" s="5">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38" s="5">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="5">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B42" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="5">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" s="5">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B46" s="5">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B47" s="5">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48" s="5">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" s="5">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" s="5">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B51" s="5">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B52" s="5">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B54" s="5">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B55" s="5">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56" s="5">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B57" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B58" s="5">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B59" s="5">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B60" s="5">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" s="5">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62" s="5">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63" s="5">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B64" s="5">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B65" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B66" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B67" s="5">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B68" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B69" s="5">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B70" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B71" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B72" s="5">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B73" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B74" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B75" s="5">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B76" s="5">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B77" s="5">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B78" s="5">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B79" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B80" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B81" s="5">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B82" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B83" s="5">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B84" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B85" s="5">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B86" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B87" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B88" s="5">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B89" s="5">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B90" s="5">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B91" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B92" s="5">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B93" s="5">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B94" s="5">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B95" s="5">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B96" s="5">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B97" s="5">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B98" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B99" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B100" s="5">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B101" s="5">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B102" s="5">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B103" s="5">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B104" s="5">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B105" s="5">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B106" s="5">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B107" s="5">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B108" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B109" s="5">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B110" s="5">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B111" s="5">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B112" s="5">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B113" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B114" s="5">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B115" s="5">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B116" s="5">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B117" s="5">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B118" s="5">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B119" s="5">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B120" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B121" s="5">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B122" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B123" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B124" s="5">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B125" s="5">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B126" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B127" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B128" s="5">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B129" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B130" s="5">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B131" s="5">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B132" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B133" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>